<commit_message>
Update region table file
</commit_message>
<xml_diff>
--- a/region_table/DEU_PDR_region_table.xlsx
+++ b/region_table/DEU_PDR_region_table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="163">
   <si>
     <t>Use</t>
   </si>
@@ -439,6 +439,75 @@
   </si>
   <si>
     <t>set</t>
+  </si>
+  <si>
+    <t>more images</t>
+  </si>
+  <si>
+    <t>weitere Bilder</t>
+  </si>
+  <si>
+    <t>mehr Bilder</t>
+  </si>
+  <si>
+    <t>Reihenfolge festzulegen</t>
+  </si>
+  <si>
+    <t>Reihenfolge zu arrangieren</t>
+  </si>
+  <si>
+    <t>arrange their order</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>information</t>
+  </si>
+  <si>
+    <t>Starten</t>
+  </si>
+  <si>
+    <t>Informationen</t>
+  </si>
+  <si>
+    <t>Fokus</t>
+  </si>
+  <si>
+    <t>anfangen</t>
+  </si>
+  <si>
+    <t>informieren</t>
+  </si>
+  <si>
+    <t>fokussieren</t>
+  </si>
+  <si>
+    <t>Start &amp; End Frames</t>
+  </si>
+  <si>
+    <t>Anfangs- und Endframe</t>
+  </si>
+  <si>
+    <t>you'd like to keep</t>
+  </si>
+  <si>
+    <t>die Sie...behalten möchten</t>
+  </si>
+  <si>
+    <t>die Sie behalten möchten</t>
+  </si>
+  <si>
+    <t>We recommend downloading the ones</t>
+  </si>
+  <si>
+    <t>Wir empfehlen diejenigen herunterzuladen</t>
+  </si>
+  <si>
+    <t>Wir empfehlen, diejenigen…herunterzuladen</t>
+  </si>
+  <si>
+    <t>Anfangs- &amp; End-Frames</t>
   </si>
 </sst>
 </file>
@@ -781,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,7 +1380,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>117</v>
       </c>
@@ -1322,7 +1391,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>120</v>
       </c>
@@ -1333,7 +1402,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>123</v>
       </c>
@@ -1344,7 +1413,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>125</v>
       </c>
@@ -1355,7 +1424,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>128</v>
       </c>
@@ -1365,8 +1434,104 @@
       <c r="C53" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>